<commit_message>
working on resizeRowToContents on editor close
</commit_message>
<xml_diff>
--- a/content_engineer_studio/testing.xlsx
+++ b/content_engineer_studio/testing.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Me\Dropbox\Python\Content Engineer Studio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Me\Dropbox\Python\content_engineer_studio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D9483C6-F4B3-412B-9524-BC853F87BCD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C3798E2-7956-4F47-B0AC-DFFA9FEA6CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="756" windowWidth="14244" windowHeight="7776" xr2:uid="{F7E6B734-54B9-435D-8347-4E48591D8B7F}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="396" windowWidth="22104" windowHeight="12660" xr2:uid="{F7E6B734-54B9-435D-8347-4E48591D8B7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>